<commit_message>
Versão 1.0.1: Atualizando código particionado
</commit_message>
<xml_diff>
--- a/data/investimentos.xlsx
+++ b/data/investimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Antera\Primatech_Analyzer v_1.0.3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090FC7CF-E70D-46DB-B236-181A6450F38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55278B8-F8E0-4C15-B9AF-FCA6FBB0FF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Empresa</t>
   </si>
@@ -202,13 +202,7 @@
     <t>12/05/23</t>
   </si>
   <si>
-    <t>Write-off</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
+    <t>Múltiplo</t>
   </si>
 </sst>
 </file>
@@ -275,12 +269,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +586,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +598,7 @@
     <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,7 +623,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -651,8 +649,8 @@
       <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
-        <v>61</v>
+      <c r="H2" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -677,8 +675,8 @@
       <c r="G3" t="s">
         <v>46</v>
       </c>
-      <c r="H3" t="s">
-        <v>62</v>
+      <c r="H3" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -703,8 +701,8 @@
       <c r="G4" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s">
-        <v>62</v>
+      <c r="H4" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,8 +727,8 @@
       <c r="G5" t="s">
         <v>48</v>
       </c>
-      <c r="H5" t="s">
-        <v>62</v>
+      <c r="H5" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -755,8 +753,8 @@
       <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
-        <v>62</v>
+      <c r="H6" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -781,8 +779,8 @@
       <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" t="s">
-        <v>62</v>
+      <c r="H7" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -807,8 +805,8 @@
       <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" t="s">
-        <v>62</v>
+      <c r="H8" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -833,8 +831,8 @@
       <c r="G9" t="s">
         <v>52</v>
       </c>
-      <c r="H9" t="s">
-        <v>62</v>
+      <c r="H9" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -859,8 +857,8 @@
       <c r="G10" t="s">
         <v>53</v>
       </c>
-      <c r="H10" t="s">
-        <v>62</v>
+      <c r="H10" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -885,8 +883,8 @@
       <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="H11" t="s">
-        <v>62</v>
+      <c r="H11" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -911,8 +909,8 @@
       <c r="G12" t="s">
         <v>55</v>
       </c>
-      <c r="H12" t="s">
-        <v>62</v>
+      <c r="H12" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -937,8 +935,8 @@
       <c r="G13" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>62</v>
+      <c r="H13" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -963,8 +961,8 @@
       <c r="G14" t="s">
         <v>57</v>
       </c>
-      <c r="H14" t="s">
-        <v>62</v>
+      <c r="H14" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -989,8 +987,8 @@
       <c r="G15" t="s">
         <v>58</v>
       </c>
-      <c r="H15" t="s">
-        <v>62</v>
+      <c r="H15" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1015,8 +1013,8 @@
       <c r="G16" t="s">
         <v>59</v>
       </c>
-      <c r="H16" t="s">
-        <v>62</v>
+      <c r="H16" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1041,8 +1039,8 @@
       <c r="G17" t="s">
         <v>44</v>
       </c>
-      <c r="H17" t="s">
-        <v>62</v>
+      <c r="H17" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>